<commit_message>
update first test cases.
</commit_message>
<xml_diff>
--- a/Energy community potential model/_calibration_results.xlsx
+++ b/Energy community potential model/_calibration_results.xlsx
@@ -5333,28 +5333,28 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>0.6515763952336627</v>
+        <v>0.66452670139884</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>0.6068839285133948</v>
+        <v>0.570709460791187</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>0.014723472288393158</v>
+        <v>0.006719362411154099</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>0.7469121300196152</v>
+        <v>0.7482047605233021</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>0.004490775699395928</v>
+        <v>0.002669371747550166</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>67.87686619949575</v>
+        <v>160.8880000132397</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>318.83759069343813</v>
+        <v>278.83759069343813</v>
       </c>
       <c r="I2" t="n" s="0">
-        <v>299.7688502299327</v>
+        <v>1481.5731635072193</v>
       </c>
     </row>
     <row r="3">
@@ -5362,28 +5362,28 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>0.6515763952336627</v>
+        <v>0.66452670139884</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>0.6068839285133948</v>
+        <v>0.570709460791187</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>0.014723472288393158</v>
+        <v>0.006719362411154099</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>0.7469121300196152</v>
+        <v>0.7482047605233021</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>0.004490775699395928</v>
+        <v>0.002669371747550166</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>150.87823090652833</v>
+        <v>84.25174345921872</v>
       </c>
       <c r="H3" t="n" s="0">
-        <v>413.8375906934381</v>
+        <v>450.8375906934381</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>1186.5731635072193</v>
+        <v>1419.5731635072193</v>
       </c>
     </row>
     <row r="4">
@@ -5391,28 +5391,28 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>0.6515763952336627</v>
+        <v>0.66452670139884</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>0.6068839285133948</v>
+        <v>0.570709460791187</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>0.014723472288393158</v>
+        <v>0.006719362411154099</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>0.7469121300196152</v>
+        <v>0.7482047605233021</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>0.004490775699395928</v>
+        <v>0.002669371747550166</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>62.09327568747551</v>
+        <v>318.1110071371959</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>186.86582996858436</v>
+        <v>241.8375906934381</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>280.42448103380605</v>
+        <v>2445.5731635072193</v>
       </c>
     </row>
     <row r="5">
@@ -5420,28 +5420,28 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>0.6515763952336627</v>
+        <v>0.66452670139884</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>0.6068839285133948</v>
+        <v>0.570709460791187</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>0.014723472288393158</v>
+        <v>0.006719362411154099</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>0.7469121300196152</v>
+        <v>0.7482047605233021</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>0.004490775699395928</v>
+        <v>0.002669371747550166</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>61.26819896540803</v>
+        <v>300.56008077866136</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>124.53800145037394</v>
+        <v>256.8375906934381</v>
       </c>
       <c r="I5" t="n" s="0">
-        <v>215.32070967619217</v>
+        <v>1376.5731635072198</v>
       </c>
     </row>
     <row r="6">
@@ -5449,28 +5449,28 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>0.6515763952336627</v>
+        <v>0.66452670139884</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>0.6068839285133948</v>
+        <v>0.570709460791187</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>0.014723472288393158</v>
+        <v>0.006719362411154099</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>0.7469121300196152</v>
+        <v>0.7482047605233021</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>0.004490775699395928</v>
+        <v>0.002669371747550166</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>63.16253729630747</v>
+        <v>43.31081446741558</v>
       </c>
       <c r="H6" t="n" s="0">
         <v>224.86582996858436</v>
       </c>
       <c r="I6" t="n" s="0">
-        <v>376.7222381012708</v>
+        <v>359.7222381012708</v>
       </c>
     </row>
     <row r="7">
@@ -5478,28 +5478,28 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n" s="0">
-        <v>0.6515763952336627</v>
+        <v>0.66452670139884</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>0.6068839285133948</v>
+        <v>0.570709460791187</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>0.014723472288393158</v>
+        <v>0.006719362411154099</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>0.7469121300196152</v>
+        <v>0.7482047605233021</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>0.004490775699395928</v>
+        <v>0.002669371747550166</v>
       </c>
       <c r="G7" t="n" s="0">
-        <v>69.0627035458209</v>
+        <v>53.32848092199182</v>
       </c>
       <c r="H7" t="n" s="0">
-        <v>116.53800145037394</v>
+        <v>224.86582996858436</v>
       </c>
       <c r="I7" t="n" s="0">
-        <v>235.32070967619217</v>
+        <v>384.7222381012708</v>
       </c>
     </row>
     <row r="8">
@@ -5507,28 +5507,28 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n" s="0">
-        <v>0.6515763952336627</v>
+        <v>0.66452670139884</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>0.6068839285133948</v>
+        <v>0.570709460791187</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>0.014723472288393158</v>
+        <v>0.006719362411154099</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>0.7469121300196152</v>
+        <v>0.7482047605233021</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>0.004490775699395928</v>
+        <v>0.002669371747550166</v>
       </c>
       <c r="G8" t="n" s="0">
-        <v>57.03463837134103</v>
+        <v>45.51312748238743</v>
       </c>
       <c r="H8" t="n" s="0">
-        <v>224.86582996858436</v>
+        <v>129.53800145037394</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>334.7222381012708</v>
+        <v>119.16336474318273</v>
       </c>
     </row>
     <row r="9">
@@ -5536,28 +5536,28 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>0.6515763952336627</v>
+        <v>0.66452670139884</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>0.6068839285133948</v>
+        <v>0.570709460791187</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>0.014723472288393158</v>
+        <v>0.006719362411154099</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>0.7469121300196152</v>
+        <v>0.7482047605233021</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>0.004490775699395928</v>
+        <v>0.002669371747550166</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>64.28697141055244</v>
+        <v>66.4505578189251</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>277.83759069343813</v>
+        <v>123.97491422516453</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>753.5731635072194</v>
+        <v>348.5731635072195</v>
       </c>
     </row>
     <row r="10">
@@ -5565,28 +5565,28 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n" s="0">
-        <v>0.6820980548229217</v>
+        <v>0.6954547692866861</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>0.5987600360056925</v>
+        <v>0.613856981848887</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>0.009274080745927806</v>
+        <v>0.013609497560717825</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>0.7088610992193948</v>
+        <v>0.8599495921873515</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>0.003605597278145101</v>
+        <v>0.0023740572741041775</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>146.58166906849812</v>
+        <v>410.92955810706303</v>
       </c>
       <c r="H10" t="n" s="0">
-        <v>449.8375906934381</v>
+        <v>447.8375906934381</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>1316.5731635072193</v>
+        <v>6025.57316350722</v>
       </c>
     </row>
     <row r="11">
@@ -5594,28 +5594,28 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n" s="0">
-        <v>0.6820980548229217</v>
+        <v>0.6954547692866861</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>0.5987600360056925</v>
+        <v>0.613856981848887</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>0.009274080745927806</v>
+        <v>0.013609497560717825</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>0.7088610992193948</v>
+        <v>0.8599495921873515</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>0.003605597278145101</v>
+        <v>0.0023740572741041775</v>
       </c>
       <c r="G11" t="n" s="0">
-        <v>68.18761136848535</v>
+        <v>47.05695144397407</v>
       </c>
       <c r="H11" t="n" s="0">
-        <v>73.8375906934381</v>
+        <v>251.8375906934381</v>
       </c>
       <c r="I11" t="n" s="0">
-        <v>187.57316350721948</v>
+        <v>416.5731635072194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>